<commit_message>
linear regression pipeline complete with the comparision between rust and python linear regression model
</commit_message>
<xml_diff>
--- a/results/Linear_regression_Result.csv.xlsx
+++ b/results/Linear_regression_Result.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\OneDrive\Desktop\Rust-Projects\ML_ALGO_Rewite\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E7926A-7E74-4737-A81C-3812F3044AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858D2885-9234-4929-A779-C6754212538A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6976E389-9B15-4863-9C6F-A420B4E4D424}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>DATASET</t>
   </si>
@@ -73,19 +73,34 @@
   </si>
   <si>
     <t>9.515 ms</t>
+  </si>
+  <si>
+    <t>Rust MSE</t>
+  </si>
+  <si>
+    <t>24.043 ms</t>
+  </si>
+  <si>
+    <t>1.565 ms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7CA668"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,8 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +445,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
@@ -487,14 +505,26 @@
       <c r="B2">
         <v>0.6139</v>
       </c>
+      <c r="C2" s="1">
+        <v>0.65098400000000001</v>
+      </c>
       <c r="D2">
         <v>505965033.1261</v>
       </c>
+      <c r="E2" s="1">
+        <v>4606896512.2850199</v>
+      </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H2" t="s">
         <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
all testing completed for linear Regression for rust vs python linear regression completed
</commit_message>
<xml_diff>
--- a/results/Linear_regression_Result.csv.xlsx
+++ b/results/Linear_regression_Result.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\OneDrive\Desktop\Rust-Projects\ML_ALGO_Rewite\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858D2885-9234-4929-A779-C6754212538A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8545B3BE-619E-427C-9F4C-3C2B5D8B3AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6976E389-9B15-4863-9C6F-A420B4E4D424}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>DATASET</t>
   </si>
@@ -82,6 +82,87 @@
   </si>
   <si>
     <t>1.565 ms</t>
+  </si>
+  <si>
+    <t>Boston Housing Dataset</t>
+  </si>
+  <si>
+    <t>1.733 ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.343 ms</t>
+  </si>
+  <si>
+    <t>24.667 ms</t>
+  </si>
+  <si>
+    <t>1.380 ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rust Predict Time </t>
+  </si>
+  <si>
+    <t>Auto MPG Dataset</t>
+  </si>
+  <si>
+    <t>0.274 ms</t>
+  </si>
+  <si>
+    <t>2.064 ms</t>
+  </si>
+  <si>
+    <t>Advertising Dataset</t>
+  </si>
+  <si>
+    <t>1.298 ms</t>
+  </si>
+  <si>
+    <t>0.245 ms</t>
+  </si>
+  <si>
+    <t>Diabetes Dataset</t>
+  </si>
+  <si>
+    <t>1.548 ms</t>
+  </si>
+  <si>
+    <t>0.252 ms</t>
+  </si>
+  <si>
+    <t>2.584 ms</t>
+  </si>
+  <si>
+    <t>0.512 ms</t>
+  </si>
+  <si>
+    <t>0.497 ms</t>
+  </si>
+  <si>
+    <t>0.841 ms</t>
+  </si>
+  <si>
+    <t>0.025 ms</t>
+  </si>
+  <si>
+    <t>0.331 ms</t>
+  </si>
+  <si>
+    <t>0.028 ms</t>
+  </si>
+  <si>
+    <t>1.191 ms</t>
+  </si>
+  <si>
+    <t>0.054 ms</t>
+  </si>
+  <si>
+    <t>Stock Market Dataset</t>
+  </si>
+  <si>
+    <t>0.098 ms</t>
+  </si>
+  <si>
+    <t>1.267 ms</t>
   </si>
 </sst>
 </file>
@@ -442,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB971067-7E0B-4BBE-8284-EA6351CE5BCC}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +570,7 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -521,7 +602,7 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>15</v>
@@ -531,6 +612,157 @@
       </c>
       <c r="K2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>-0.1779</v>
+      </c>
+      <c r="C3">
+        <v>0.58426999999999996</v>
+      </c>
+      <c r="D3">
+        <v>31.671299999999999</v>
+      </c>
+      <c r="E3">
+        <v>4466072770.7544003</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>0.212492825720139</v>
+      </c>
+      <c r="C4">
+        <v>0.57030999999999998</v>
+      </c>
+      <c r="D4">
+        <v>28.2358224073324</v>
+      </c>
+      <c r="E4">
+        <v>14.549307000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>0.90247132416945797</v>
+      </c>
+      <c r="C5">
+        <v>0.87556299999999998</v>
+      </c>
+      <c r="D5">
+        <v>2.6369407160816101</v>
+      </c>
+      <c r="E5">
+        <v>3.0560689999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>0.299000777026311</v>
+      </c>
+      <c r="C6">
+        <v>0.25683299999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.16094369915212201</v>
+      </c>
+      <c r="E6">
+        <v>0.169215</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>0.32612154927842202</v>
+      </c>
+      <c r="C7">
+        <v>-0.20691899999999999</v>
+      </c>
+      <c r="D7">
+        <v>5070387311095220</v>
+      </c>
+      <c r="E7">
+        <v>7412450837751620</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>